<commit_message>
Updated All Menu & Help
</commit_message>
<xml_diff>
--- a/src/test/resource/Datasheets/AmazonDataSheet.xlsx
+++ b/src/test/resource/Datasheets/AmazonDataSheet.xlsx
@@ -1,18 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27510"/>
+  <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anuimtiaz/git/AmazonProject/src/test/resource/Datasheets/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="23910" windowHeight="6465"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420"/>
   </bookViews>
   <sheets>
     <sheet name="AmazonDataSheet" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1:X20"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -55,7 +67,7 @@
     <t>Laptop</t>
   </si>
   <si>
-    <t>Guitar</t>
+    <t>Shoes</t>
   </si>
 </sst>
 </file>
@@ -157,12 +169,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -192,12 +204,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -401,18 +413,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -420,7 +432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -428,7 +440,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -436,7 +448,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -444,7 +456,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -452,7 +464,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -460,7 +472,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -468,7 +480,6 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -480,7 +491,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -492,7 +503,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>